<commit_message>
residuals and RMSE added to OLS
</commit_message>
<xml_diff>
--- a/Week 8 - Analysis/JC/OLS Results.xlsx
+++ b/Week 8 - Analysis/JC/OLS Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Repos\culminating-project-group-1\Week 8 - Analysis\JC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D741BC31-2CF8-4E07-A546-E16F12486B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AB2E9A-A8D6-452B-B230-CCC6EF408FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model Fit" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="129">
   <si>
     <t>Variable</t>
   </si>
@@ -423,12 +423,18 @@
   </si>
   <si>
     <t>Incidence of tuberculosis</t>
+  </si>
+  <si>
+    <t>RMSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -490,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -521,6 +527,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,6 +552,310 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -638,6 +951,25 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -658,329 +990,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1265,8 +1274,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5E236484-4D8B-4641-AE1E-A979E43FCE28}" name="Table6" displayName="Table6" ref="A1:D13" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
-  <autoFilter ref="A1:D13" xr:uid="{5E236484-4D8B-4641-AE1E-A979E43FCE28}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5E236484-4D8B-4641-AE1E-A979E43FCE28}" name="Table6" displayName="Table6" ref="A1:D14" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+  <autoFilter ref="A1:D14" xr:uid="{5E236484-4D8B-4641-AE1E-A979E43FCE28}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{972B2640-1556-4A03-869F-BCA6181458DD}" name=" Statistic                           " dataDxfId="35"/>
     <tableColumn id="2" xr3:uid="{1F473E26-DFD9-4CCA-A2D4-5B32D90260E6}" name=" Environmental Model         " dataDxfId="34"/>
@@ -1296,54 +1305,54 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A9C9FE16-118C-4ECA-A431-90E77AC7C113}" name="Table8" displayName="Table8" ref="A2:F24" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A9C9FE16-118C-4ECA-A431-90E77AC7C113}" name="Table8" displayName="Table8" ref="A2:F24" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A2:F24" xr:uid="{A9C9FE16-118C-4ECA-A431-90E77AC7C113}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F24">
     <sortCondition descending="1" ref="B2:B24"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{AB27E42D-219F-4B19-AEDE-8A769B508823}" name="Variable" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{4D74A56B-9475-4F58-B368-18CB8F03A8B2}" name="Coefficient" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{9D885BE2-7269-4483-9071-5CB1F9169DD7}" name="Std Err" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{40A4309A-D46D-48EF-8D57-0FA1785F7ABF}" name="t" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{D87A07D1-9866-4BB7-8A58-35F9913F8BBE}" name="P-value" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{57528BC9-FDCE-4D9E-A54D-830654B27FEA}" name="95% CI" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{AB27E42D-219F-4B19-AEDE-8A769B508823}" name="Variable" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{4D74A56B-9475-4F58-B368-18CB8F03A8B2}" name="Coefficient" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{9D885BE2-7269-4483-9071-5CB1F9169DD7}" name="Std Err" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{40A4309A-D46D-48EF-8D57-0FA1785F7ABF}" name="t" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{D87A07D1-9866-4BB7-8A58-35F9913F8BBE}" name="P-value" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{57528BC9-FDCE-4D9E-A54D-830654B27FEA}" name="95% CI" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9ACCC06E-E512-453D-B51B-B8BCC4998739}" name="Table9" displayName="Table9" ref="A2:F12" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9ACCC06E-E512-453D-B51B-B8BCC4998739}" name="Table9" displayName="Table9" ref="A2:F12" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A2:F12" xr:uid="{9ACCC06E-E512-453D-B51B-B8BCC4998739}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F12">
     <sortCondition descending="1" ref="B2:B12"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F57647CD-C35C-44A8-BA70-3A24135A7A0F}" name="Variable" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{D68751F5-337B-44C2-8C38-FF774F87868F}" name="Coefficient" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{FE94608F-EB64-4768-A406-2276A2B7FA09}" name="Std Err" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{C4CB1CF5-4BB6-4526-B8F1-34F72BE9FDA5}" name="t" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{09AF57B6-3B75-4AFD-9237-F6DF63E1CC22}" name="P-value" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{DDBE05EA-500D-44B2-ACD3-BCBE316EBDE6}" name="95% CI" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{F57647CD-C35C-44A8-BA70-3A24135A7A0F}" name="Variable" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{D68751F5-337B-44C2-8C38-FF774F87868F}" name="Coefficient" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{FE94608F-EB64-4768-A406-2276A2B7FA09}" name="Std Err" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{C4CB1CF5-4BB6-4526-B8F1-34F72BE9FDA5}" name="t" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{09AF57B6-3B75-4AFD-9237-F6DF63E1CC22}" name="P-value" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{DDBE05EA-500D-44B2-ACD3-BCBE316EBDE6}" name="95% CI" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{C16E03D5-E60B-46C2-9C8D-5C7BD8CAFF0A}" name="Table911" displayName="Table911" ref="A15:F25" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{C16E03D5-E60B-46C2-9C8D-5C7BD8CAFF0A}" name="Table911" displayName="Table911" ref="A15:F25" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A15:F25" xr:uid="{C16E03D5-E60B-46C2-9C8D-5C7BD8CAFF0A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:F25">
     <sortCondition descending="1" ref="B2:B12"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{399321A8-D8FC-492A-B904-EA5964EC209F}" name="Variable" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{24F1FCFC-F2FF-4044-B85E-BF9D1C8D52FA}" name="Coefficient" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{2A30F612-19B2-4E48-892A-A26A4A6F5A20}" name="Std Err" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{D5F37563-866B-4EF3-96E9-1FECF0C72F12}" name="t" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{66B94B2E-AEBD-4DEE-B267-A50D1A5C0684}" name="P-value" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{6EBB910C-A553-4C8B-A098-F03FF67E6756}" name="95% CI" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{399321A8-D8FC-492A-B904-EA5964EC209F}" name="Variable" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{24F1FCFC-F2FF-4044-B85E-BF9D1C8D52FA}" name="Coefficient" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{2A30F612-19B2-4E48-892A-A26A4A6F5A20}" name="Std Err" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{D5F37563-866B-4EF3-96E9-1FECF0C72F12}" name="t" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{66B94B2E-AEBD-4DEE-B267-A50D1A5C0684}" name="P-value" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{6EBB910C-A553-4C8B-A098-F03FF67E6756}" name="95% CI" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1612,10 +1621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D6CA7E1-9CA8-477F-89AB-0A3299EE2523}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:D13"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1711,99 +1720,113 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="4">
-        <v>252.4</v>
-      </c>
-      <c r="C7" s="4">
-        <v>453.3</v>
-      </c>
-      <c r="D7" s="7">
-        <v>1704</v>
+        <v>128</v>
+      </c>
+      <c r="B7" s="12">
+        <v>23.917000000000002</v>
+      </c>
+      <c r="C7" s="12">
+        <v>15.439490694179399</v>
+      </c>
+      <c r="D7" s="12">
+        <v>8.9317796639129803</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>56</v>
+        <v>33</v>
+      </c>
+      <c r="B8" s="4">
+        <v>252.4</v>
+      </c>
+      <c r="C8" s="4">
+        <v>453.3</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1704</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="8">
-        <v>-6912.8</v>
-      </c>
-      <c r="C9" s="8">
-        <v>-6280.1</v>
-      </c>
-      <c r="D9" s="8">
-        <v>-5716.3</v>
+        <v>34</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="7">
-        <v>13860</v>
-      </c>
-      <c r="C10" s="7">
-        <v>12600</v>
-      </c>
-      <c r="D10" s="7">
-        <v>11450</v>
+        <v>35</v>
+      </c>
+      <c r="B10" s="8">
+        <v>-6912.8</v>
+      </c>
+      <c r="C10" s="8">
+        <v>-6280.1</v>
+      </c>
+      <c r="D10" s="8">
+        <v>-5716.3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="7">
-        <v>13970</v>
+        <v>13860</v>
       </c>
       <c r="C11" s="7">
-        <v>12730</v>
+        <v>12600</v>
       </c>
       <c r="D11" s="7">
-        <v>11520</v>
+        <v>11450</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="4">
-        <v>18</v>
-      </c>
-      <c r="C12" s="4">
-        <v>21</v>
-      </c>
-      <c r="D12" s="4">
-        <v>10</v>
+        <v>37</v>
+      </c>
+      <c r="B12" s="7">
+        <v>13970</v>
+      </c>
+      <c r="C12" s="7">
+        <v>12730</v>
+      </c>
+      <c r="D12" s="7">
+        <v>11520</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="4">
+        <v>18</v>
+      </c>
+      <c r="C13" s="4">
+        <v>21</v>
+      </c>
+      <c r="D13" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B14" s="7">
         <v>2289</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C14" s="7">
         <v>2286</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D14" s="7">
         <v>2297</v>
       </c>
     </row>
@@ -1820,7 +1843,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F21"/>
+      <selection activeCell="A4" sqref="A4:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2261,8 +2284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C002A61-CA7C-445D-A5BF-F9F38721554D}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F24"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>